<commit_message>
fixed use_link reading when form is not valid
</commit_message>
<xml_diff>
--- a/sample(no online class).xlsx
+++ b/sample(no online class).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="시간표" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>8:50~9:40</t>
   </si>
@@ -173,10 +173,7 @@
     <t>이 워크시트의 데이터로 시간표가 만들어짐</t>
   </si>
   <si>
-    <t>&lt;- 왼쪽 표에 교실 입력하면 자동으로 생성됨</t>
-  </si>
-  <si>
-    <t>링크</t>
+    <t>&lt;- 왼쪽 표에 교실을 입력하면 자동으로 생성됨</t>
   </si>
   <si>
     <t>https://ksatimetable.herokuapp.com</t>
@@ -738,9 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1080,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1091,7 +1086,7 @@
     <col min="5" max="5" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1105,12 +1100,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1119,12 +1114,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1133,12 +1128,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1147,12 +1142,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1161,12 +1156,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -1175,12 +1170,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1189,12 +1184,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -1203,12 +1198,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -1217,12 +1212,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1231,7 +1226,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E11" s="11" t="s">
         <v>29</v>
       </c>
@@ -1239,12 +1234,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E12" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E13" s="14" t="s">
         <v>30</v>
       </c>
@@ -1252,24 +1247,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="F14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F14" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="15" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F15" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="F15" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G14" r:id="rId1"/>
+    <hyperlink ref="F14" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>